<commit_message>
Add all svm data
</commit_message>
<xml_diff>
--- a/LaTex/data/svm_lineal_k.xlsx
+++ b/LaTex/data/svm_lineal_k.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Train" sheetId="1" r:id="rId1"/>
+    <sheet name="Train" sheetId="2" r:id="rId1"/>
+    <sheet name="Validation" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
   <si>
     <t>affirmative</t>
   </si>
@@ -391,10 +392,517 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:X14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2532</v>
+      </c>
+      <c r="D3">
+        <v>85</v>
+      </c>
+      <c r="E3">
+        <v>63</v>
+      </c>
+      <c r="F3">
+        <v>56</v>
+      </c>
+      <c r="G3">
+        <v>39</v>
+      </c>
+      <c r="H3">
+        <v>94</v>
+      </c>
+      <c r="I3">
+        <v>69</v>
+      </c>
+      <c r="J3">
+        <v>44</v>
+      </c>
+      <c r="K3">
+        <v>122</v>
+      </c>
+      <c r="L3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>46</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>120</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>75</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>75</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>99</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>70</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>42</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3">
+        <f>C3</f>
+        <v>2532</v>
+      </c>
+      <c r="D13" s="3">
+        <f>D4</f>
+        <v>46</v>
+      </c>
+      <c r="E13" s="3">
+        <f>E5</f>
+        <v>100</v>
+      </c>
+      <c r="F13" s="3">
+        <f>F6</f>
+        <v>120</v>
+      </c>
+      <c r="G13" s="3">
+        <f>G7</f>
+        <v>75</v>
+      </c>
+      <c r="H13" s="3">
+        <f>H8</f>
+        <v>75</v>
+      </c>
+      <c r="I13" s="3">
+        <f>I9</f>
+        <v>99</v>
+      </c>
+      <c r="J13" s="3">
+        <f>J10</f>
+        <v>70</v>
+      </c>
+      <c r="K13" s="3">
+        <f>K11</f>
+        <v>42</v>
+      </c>
+      <c r="L13" s="3">
+        <f>L12</f>
+        <v>109</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3">
+        <f>SUM(C3:C12) - C13</f>
+        <v>42</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" ref="D14:L14" si="0">SUM(D3:D12) - D13</f>
+        <v>94</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>